<commit_message>
Corrección header, capacitores y resistencias
</commit_message>
<xml_diff>
--- a/Documentación SIWA/SIWA BOM Excel Lista de componentes.xlsx
+++ b/Documentación SIWA/SIWA BOM Excel Lista de componentes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\Altium\Proyecto integrador\SIWA PCB\Project Outputs for SIWA PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B2F72D-561C-4911-929E-A5A0BB7D34EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58EEEF87-BBA8-4F04-9A9A-6355133C6285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{9E122235-7502-418F-A27E-1860EC358426}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{BC4F0531-A7D7-48AB-B5D5-E0CC4A465226}"/>
   </bookViews>
   <sheets>
     <sheet name="SIWA BOM Excel Lista de compone" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <t>61200821621</t>
   </si>
   <si>
-    <t>Alimentacion, HeaderLEDs, LCD</t>
+    <t>Alimentacion, LCD</t>
   </si>
   <si>
     <t>CMP-1502-00006-2</t>
@@ -773,7 +773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914CEC6-3231-4B45-9B82-AD9BE1099CC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060081C7-01CE-484D-84A7-F58BA482AB19}">
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -865,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>21</v>
@@ -886,7 +886,7 @@
         <v>0.97</v>
       </c>
       <c r="O2" s="1">
-        <v>2.91</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
         <v>56</v>
       </c>
       <c r="N8" s="1">
-        <v>0.17953</v>
+        <v>0.17979000000000001</v>
       </c>
       <c r="O8" s="1">
         <v>1.8</v>
@@ -1401,10 +1401,10 @@
         <v>86</v>
       </c>
       <c r="N14" s="1">
-        <v>9.8699999999999996E-2</v>
+        <v>8.9700000000000002E-2</v>
       </c>
       <c r="O14" s="1">
-        <v>9.8699999999999996E-2</v>
+        <v>8.9700000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>